<commit_message>
fix bug method "checkID"
</commit_message>
<xml_diff>
--- a/bin/Debug/net6.0/ClientInfo.xlsx
+++ b/bin/Debug/net6.0/ClientInfo.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <d:rPr>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>1234</t>
   </si>
   <si>
     <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
@@ -141,7 +147,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -178,6 +184,34 @@
         <v>23</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>359</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>160</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="0">
+        <v>1234</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>
@@ -185,7 +219,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="B1:C2"/>
+  <dimension ref="B1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -193,10 +227,10 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2">
@@ -205,6 +239,22 @@
       </c>
       <c r="C2" s="0" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new Class (ExcelMethodGroup) with new method for work with excelFile
</commit_message>
<xml_diff>
--- a/bin/Debug/net6.0/ClientInfo.xlsx
+++ b/bin/Debug/net6.0/ClientInfo.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <d:rPr>
@@ -65,13 +65,13 @@
     </d:r>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>1234</t>
+    <t>MIKHAIL</t>
+  </si>
+  <si>
+    <t>NOVIKAU</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
   <si>
     <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
@@ -92,6 +92,12 @@
       </d:rPr>
       <d:t xml:space="preserve">Password</d:t>
     </d:r>
+  </si>
+  <si>
+    <t>MELMENX</t>
+  </si>
+  <si>
+    <t>2127979Z</t>
   </si>
 </sst>
 </file>
@@ -147,7 +153,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -172,44 +178,36 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="0">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="E2" s="0">
+        <v>30001</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>359</v>
+        <v>1449</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="0">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0">
-        <v>160</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="0">
-        <v>1234</v>
+        <v>25</v>
+      </c>
+      <c r="E3" s="0">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -219,7 +217,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="B1:C4"/>
+  <dimension ref="B1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -235,25 +233,17 @@
     </row>
     <row r="2">
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="0" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>